<commit_message>
Se eliminan datos sensibles
</commit_message>
<xml_diff>
--- a/report/reporte_asistencia_v2.xlsx
+++ b/report/reporte_asistencia_v2.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flasa\OneDrive\Escritorio\back-checador\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6450063-37B1-463E-B0EB-F3F6B7256FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9DB6D8-71BB-4E06-9C44-6AB8B648CF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4B064F43-C61A-45ED-BD97-54BFAB11C60D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4B064F43-C61A-45ED-BD97-54BFAB11C60D}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Nombre</t>
   </si>
@@ -52,12 +53,18 @@
   <si>
     <t>Extra</t>
   </si>
+  <si>
+    <t>Comida</t>
+  </si>
+  <si>
+    <t>Dia</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +77,13 @@
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -97,19 +111,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -149,6 +166,55 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAE4FCD6-4A42-475B-A993-DC51EF035860}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="762000" y="219075"/>
+          <a:ext cx="1371600" cy="704850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2AA694B-076C-48E9-9276-59BAA727662D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -494,49 +560,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CCAF224-50AB-44E3-9FDF-C77D5802D840}">
-  <dimension ref="B4:I8"/>
+  <dimension ref="B4:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:H4"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
-    <col min="8" max="8" width="19.7109375" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" customWidth="1"/>
+    <col min="1" max="5" width="11.42578125" style="5"/>
+    <col min="6" max="6" width="19.140625" style="5" customWidth="1"/>
+    <col min="7" max="12" width="23.7109375" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="8" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="I8:J8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98F7AB30-D4AA-43CF-B9AC-EC79867FEFDA}">
+  <dimension ref="B4:L8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="11.42578125" style="5"/>
+    <col min="6" max="6" width="19.140625" style="5" customWidth="1"/>
+    <col min="7" max="12" width="23.7109375" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
     </row>
-    <row r="8" spans="2:9" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
+    <row r="8" spans="2:12" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
       <c r="F8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="I8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8" s="3"/>
+      <c r="K8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="L8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B8:E8"/>
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="F4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>